<commit_message>
Salavando primeira versão do projeto
</commit_message>
<xml_diff>
--- a/Auto_ML_Libs.xlsx
+++ b/Auto_ML_Libs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,110 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Biblioteca</t>
+  </si>
+  <si>
+    <t>Caracteríticas</t>
+  </si>
+  <si>
+    <t>Auto-Sklearn</t>
+  </si>
+  <si>
+    <t>Auto-Keras</t>
+  </si>
+  <si>
+    <t>Google Cloud AutoML</t>
+  </si>
+  <si>
+    <t>AutoML</t>
+  </si>
+  <si>
+    <t>Pycaret</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>TPOT</t>
+  </si>
+  <si>
+    <t>AutoGluon</t>
+  </si>
+  <si>
+    <t>DataRobot</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>Tazi.ai</t>
+  </si>
+  <si>
+    <t>JADBio AutoML</t>
+  </si>
+  <si>
+    <t>MLJar</t>
+  </si>
+  <si>
+    <t>Dataiku</t>
+  </si>
+  <si>
+    <t>Microsoft Azure AutoML</t>
+  </si>
+  <si>
+    <t>Amazon SageMaker Autopilot</t>
+  </si>
+  <si>
+    <t>Akkio</t>
+  </si>
+  <si>
+    <t>Grátis</t>
+  </si>
+  <si>
+    <t>Feature Eng</t>
+  </si>
+  <si>
+    <t>Feature Selection</t>
+  </si>
+  <si>
+    <t>Limite Tempo Processamento</t>
+  </si>
+  <si>
+    <t>Tunning</t>
+  </si>
+  <si>
+    <t>Redes Neurais</t>
+  </si>
+  <si>
+    <t>Popularidade</t>
+  </si>
+  <si>
+    <t>DataBricks AutoML</t>
+  </si>
+  <si>
+    <t>Explicação</t>
+  </si>
+  <si>
+    <t>gramas</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +215,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +250,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +432,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>3750</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>